<commit_message>
added drp_base to root config
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/vu13p_gty_root.xlsx
+++ b/examples/vu13p_25g_all/src/vu13p_gty_root.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -195,6 +195,15 @@
   </si>
   <si>
     <t xml:space="preserve">memory base for PCIe systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drp_base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x464000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRP interface base address, AXI systems only</t>
   </si>
   <si>
     <t xml:space="preserve">Instructions</t>
@@ -345,7 +354,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -367,12 +376,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -423,7 +426,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -436,11 +439,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -464,7 +463,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -657,7 +656,7 @@
       <c r="A18" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="0" t="s">
@@ -706,6 +705,17 @@
       </c>
       <c r="C22" s="0" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -787,224 +797,224 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="4" t="s">
-        <v>70</v>
+      <c r="C13" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="4" t="s">
-        <v>71</v>
+      <c r="C14" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="4" t="s">
-        <v>72</v>
+      <c r="C15" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="4" t="s">
-        <v>73</v>
+      <c r="C16" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>